<commit_message>
Get daily reddit data: Tue Jun 24 08:13:28 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_29.xlsx
+++ b/data/collected_data/2025_06_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3559 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1lj55sg</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>French tips with chrome sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpl5kjlizt8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1lj4pt7</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Loving how smooth my nails are after being filed</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pov8gd43ut8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1lj4iuv</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>I might need acrylic toenails!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lj4iuv/i_might_need_acrylic_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1lj4ddz</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Nail project</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lugisua1qt8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1lj4a34</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Another one</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj4a34</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1lj46bk</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Have you ever spent two hours prepping your nails, started painting, and realized around the seventh finger that you were using UV gel under an LED lamp?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vm187v5rnt8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1lj419i</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dznpncv4mt8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1lj3s3s</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>What shape would best suite my hands?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2v0dub58jt8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1lj3kg6</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>First time trying almond, does it look good on my hands?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj3kg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1lj2r7j</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>What shape and polish would suit me?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj2r7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1lj1z2m</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Summer nails! 🌈</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0gfe0jpzs8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1lj1xqw</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Pyrite or Gold?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx58uiubzs8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1lj1l7r</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>What to do about flat nail?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lj1l7r/what_to_do_about_flat_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1lizl0o</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Salon gel peeling on day 3, what should I ask for!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lizl0o/salon_gel_peeling_on_day_3_what_should_i_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1lj1p8e</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>freestyle I did not so long ago</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yk2y7kxws8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1lj14fw</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Did my own for an upcoming festival this weekend!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj14fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1lj0fj8</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Fill or Soak off ?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6lfm4mtks8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1lj0evq</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Cat Eye Nails &amp; White Toes 💖</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/raviq3aoks8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1lj0emy</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in a while!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2uc7e1mks8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1lj0aui</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Matching frenchies 💅❤️</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2noz16mjs8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1lizy6a</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Just showing off these amazing nails my tech did</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52mytfsfgs8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1lizpor</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>This is what I think princess nails are</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lizpor</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1liza8q</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Only second time doing my nails but I love them so much</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liza8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1liyxdm</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Burning when getting them done?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liyxdm/burning_when_getting_them_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1livk7m</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Nail Inspo 👀🐕</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsv9d9doer8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1lixtkm</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Got my nails done for a work event. Ended up quitting my job, but at least my nails looked good!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lixtkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1liyo7i</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>BIAB nail lifting</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liyo7i/biab_nail_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1liyhe0</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Pink is my favorite</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0o1iaq6h3s8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1liyc7g</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Still Learning!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xymcpkv62s8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1lixzhy</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Cute? They change color</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5djk0ht3zr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1lix5qn</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Juicy set! (i love the 3D charms🥰)</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lix5qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1liw0jh</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Cuccio milk and honey cuticle oil perfume?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liw0jh/cuccio_milk_and_honey_cuticle_oil_perfume/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1liwme0</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>First time using solid builder gel...</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liwme0</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1lix377</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>$62 and yes, I spoke up throughout. The manager is asking me to go back tomorrow so he can redo them but I think not 😅</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6hwr2earr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1lix0us</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Always Get Cut at the Nail Salon. At-Home Alternatives?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lix0us/always_get_cut_at_the_nail_salon_athome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1liwv6o</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Painting cat eye on press ons</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liwv6o/painting_cat_eye_on_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1liwpgz</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>My natural nail lifted from my nail bed</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liwpgz/my_natural_nail_lifted_from_my_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1liwpfl</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Scalloped Nails!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liwpfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1liwo5e</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Base coat on sculpture gel?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liwo5e/base_coat_on_sculpture_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1liwju3</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Is this normal at the two week mark?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbj4fqipmr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1liw1di</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Summer is here!!!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j79i92jiir8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1livtqk</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Some of my nails as a girl who likes basics with a twist!</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1livtqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1livs2s</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>nails for my camping trip (i was going to do the holdy thing with a seagull but they’re too fast)</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0f8pnm7dgr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1livqxf</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Nails for my sisters gender reveal 🩵🩷🍼</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p51oas54gr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1livopy</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets I’ve done!!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1livopy</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1livihj</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Nails that matcha</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4r9a5z3ber8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1livcqr</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Turquoise Cat Eye Nails</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/burz4642dr8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1liva69</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Never liked pink ..until now</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhp9urthcr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1liv61v</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Some mermaid glitter for the first week of summer ☀️</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liv61v</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1liuoxs</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Nails I did when I was 16. :)</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liuoxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1liuhr0</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Pretty in pink - my favorite set so far 🎀</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a06aw3ji6r8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1liudrb</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Love my nails and jewelry</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mv6uhwo5r8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1liubdl</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Help shaping nails?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liubdl/help_shaping_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1liu96l</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>This set EATS</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylyse9yp4r8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1liu8at</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>First time ever using builder gel!</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liu8at</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1litw2h</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Revel Swift Soak</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1litw2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1lith5c</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Advice on shellac polish discolouration?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lith5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1lit919</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Growth appreciation post since I’m going to have to trim them tonight I’ve been getting breaks, chips &amp; tears!  😣</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lit919</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1lit6kp</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Nails popping off</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/945g3axzwq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1listwb</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Going to f1 this weekend, did some Max Verstappen inspired nails for myself</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5lli0vfuq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1lirimb</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>My nail artist really saw my vision! Inspo from WGNails on Etsy, done by @stassisnails in Chicago</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lirimb</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1liscat</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>I did my first xxxl ✨️ExTrA✨️ set, what do we think?🫣</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liscat</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1litgut</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Orange is the vacation colour 🧡</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlvx9qg2zq8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1lit9vu</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>ring of fire or stained?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lit9vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1lisxb8</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>My nails but better, with flair</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6btiea5vq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1lis9ag</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>What would you pay for these ?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28kf78siqq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1lis5n7</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Not to everyone's taste but one of my favourite sets I've done + 22 gems</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lis5n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1lis4e9</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Today I made these super nails 🤣🤣 xxl</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va52ztzjpq8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1liruxq</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Ocean waves</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liruxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1lirl8c</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>2 Days after and it’s peeling…should i be pissed?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zslfy67wlq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1lirkpm</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>New Pedicure</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lirkpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1liqz1m</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Allergen free gel recommendations</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liqz1m/allergen_free_gel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1liquqf</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liquqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1liqm1z</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Took the plunge</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liqm1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1liqka4</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Fresh summer set</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liqka4</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1liqlby</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>First go at magnetic gel polish!</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liqlby/first_go_at_magnetic_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1liqbax</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>I put a little glitter on the nails to make them shimmer</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcd1dyaycq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1lipm9g</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lipm9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1linszv</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Press on nails for funky shape</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4we3vh0wp8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1lioauz</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>My first nails! Took me abt 6 hours. What can I do better ? (Yeah I’m in pain cuz of my cuticles 😔😭)</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lioauz</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1linbvu</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>What’s the difference?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1linbvu/whats_the_difference/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1liosuj</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Nail Supplies in DC/DMV</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liosuj/nail_supplies_in_dcdmv/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1lipj76</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Beach vacay nail slay 🏝️👙</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lipj76</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1lipi4a</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Run dont walk to dollar tree</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lipi4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1lipa10</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Summer Gel X set! 🤍🐚</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lipa10</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1lip1eh</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Help with my diy gel nails</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/969obece4q8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1lioyip</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Would you like this service or not really?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lioyip/would_you_like_this_service_or_not_really/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1lioq2z</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Junk nails!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lioq2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1lionnu</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Need diy tutorial recs!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lionnu/need_diy_tutorial_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1lioma7</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Press-On brands for large hands with flat beds</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lioma7/presson_brands_for_large_hands_with_flat_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1lioh80</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>HAPPY FACE/ PRIDE</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee9pkinl0q8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1liofy4</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Do you find any essential oils make any difference besides just smell in your nail / cuticle oils?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1liofy4/do_you_find_any_essential_oils_make_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1lio5h6</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Leopard print pink 🔥🩷</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lio5h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1lio1tc</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Thoughts on textured fish?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kdmxvj9mxp8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1linyih</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>I'll never get enough off magnetic nails 🥹</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1linyih</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1linryr</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>learning to speak up when we don’t like a service</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1linryr/learning_to_speak_up_when_we_dont_like_a_service/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1linpfw</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Summer French! Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1linpfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1lindtg</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Want to surprise my girlfriend by getting her nails done but i’m so confused i’m just a boy</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lindtg/want_to_surprise_my_girlfriend_by_getting_her/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1lindns</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>A little color</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpea9216tp8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1limzb1</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>4th of July nails!</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bh5vqqdjqp8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1lj4tqq</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>My nails are gonna hate me for swimming so much, but at least they got the right color for it ;)</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj4tqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1lj1jjz</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Mooncat with Dazzle Dry System</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kdc1p4ldvs8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1lj1dly</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Recreated ILNP Polishes</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j6ropg1tts8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1lj0blc</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Playing around with some combos</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l06yawhtjs8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1lj0alx</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Which shade would you use twice in this skittle?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svy5130kjs8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1lj073l</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Fun with thermals 😁 Holo Taco Peely Base and Glossy Taco, 3 coats of Emily De Molly A Spot In The Woods</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj073l</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1lj05br</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Pride nails!</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj05br</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1lj0220</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Linear Rainbow</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj0220</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1liyvuz</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Is there a way to do your nails like this?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja327sd17s8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1liyf3r</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>🌌O-Type Star 🌠</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liyf3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1liyarx</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>2 thermals with similar cold states, but very different warm states.</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liyarx</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1lixweq</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Space alien or mermaid?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lixweq</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1lixcy1</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Has anyone ever patched their chipped nails with a different color?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lixcy1/has_anyone_ever_patched_their_chipped_nails_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1lixbzy</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>LA Colors???</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9laccdetr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1liwunp</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>foggy polish</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6npchfapr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1liwphb</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Please share photos of your PPU Rewind 2025 polishes!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj96y5t1or8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1livvvz</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Psilocybin appreciation + a question</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1livvvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1livns8</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Summer nails ✅️</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1livns8</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1liviyl</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Name this nail polish brand--Almay or another brand?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7yiozxwdr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1livgtu</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>🗡️🔮 When Passions Collide (aka a nerdy collection of sparkly little things) [paid PR]</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yl9ik3nxdr8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1liv9u3</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time. How’d they turn out?</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nepjl6lfcr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1liv101</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Can I post about my absolute genuine disgust of AI used in the nail industry??</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08yjxdwkar8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1liubmq</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>ILNP No Days Off on my days off</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liubmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1liu0co</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Which one looks better?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liu0co</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1lityhn</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>dupe for Dany Viana Hitsuzen?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lityhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1litxun</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Tinted base coat recs $12 and under</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1litxun/tinted_base_coat_recs_12_and_under/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1littmx</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>...and fire</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/4rcHgxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1liso3i</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Hello nail polish lovers I have a question</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>/r/Nailpolish/comments/1lisnln/hello_nail_polish_lovers_i_have_a_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1lisjop</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Does anyone have this? Is it a base coat?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lisjop</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1lisdm9</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>My nails but better</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/835t9xemqq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1lis6i5</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Just me, vibing and doing my nails when it’s literally 100F and the air is thicker (and hotter?) than pea soup 🥲</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lis6i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1lis1oj</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Hi, I'm new here 😊 Storage reccommendations for beginners?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lis1oj</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1lirx2l</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Replacement for Essie’s Walk Down the Aisle?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lirx2l/replacement_for_essies_walk_down_the_aisle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1lirbi1</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Beetle Nails</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lirbi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1liqyjx</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Nail Envy</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1liqyjx/nail_envy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1liqws2</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Trop it like it's hot (Trop it like it's hot, trop it like it's hot)</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liqws2</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1liqg33</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>I did something funny! Another happy little accident!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liqg33</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1liq4x4</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>I Understand Now 😍</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qucvhl7ubq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1liq2g9</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Showing off our summer manis 💅🏼</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liq2g9</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1liq1xm</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>BKL Master of Spinning Bullshit vs Wyrd</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1liq1xm/bkl_master_of_spinning_bullshit_vs_wyrd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1liq03i</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>What shade is the base color from @yun.s_nails?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lowghdpmaq8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1lipwlz</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Builder Gel Shades in Lacquer/Polish</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lipwlz/builder_gel_shades_in_lacquerpolish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1lipwk6</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Candy wrapper skittle nails</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lipwk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1lipvi8</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>A Glitter Packed Polish 💙</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lipvi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1liptu1</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Recommendations for a base coat please.</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1liptu1/recommendations_for_a_base_coat_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1lipg83</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Super Bloom bandwagon</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lipg83</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1lip173</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Taste the Rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vm91mdd4q8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1lionqs</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Topographical map vibes?? 🗺️</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lionqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1liohd5</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Has anyone ever tried to put chrome powder over a chrome finish polish?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3c1jusym0q8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1lio9rh</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Cannot figure out what went wrong</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lio9rh</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1lin5i0</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Ppu rewind shipping cost.</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lin5i0/ppu_rewind_shipping_cost/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1limds0</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>🎶 Life is just a bowl of cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1limds0</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1lim6kg</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Compiled a little comparison of Ether Dragon "dupes" and siblings.</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lim6kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1lim0ms</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Why have I never tried holo polishes before?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jadhp6drip8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1lilzss</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Do not sleep on Aura Lacquer: "Scorpio Moon"</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hg1c0hwyjp8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1lilv9o</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>My first non-gel magnetic. It's mesmerizing!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26druin4jp8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1lilps7</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Base and top coat?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lilps7/base_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1lilgqr</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquers creator moving on to focus on their new brand “Haunted Polish”</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfk4j8mdgp8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1lileyd</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>One of the prettiest polishes I own 😍</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jl6lghzzfp8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1lilefc</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Asking for a dupe - navy blue with green shimmer from this month’s LBH</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3sqy5unfp8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1lijx54</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Sparkly purple!</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lijx54</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1lijsij</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Worst polish stain I’ve ever had</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cfs0ay35p8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1lijsbs</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Bare Naked Shorties</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sz1xlh335p8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1liijf8</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Would you rather buy 5ml nail polish or 12/15 ml?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1liijf8/would_you_rather_buy_5ml_nail_polish_or_1215_ml/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1lii9ih</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Worth the wait!</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lii9ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1lii0va</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Les BEE an pride 🌈 🐝</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lii0va</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1lihn9a</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Grown out damage?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpg286j4qo8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1lih9ao</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>So glowy ✨🛼🧚‍♀️🩵</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lih9ao</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ligvjx</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>something bright for summer :’)</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ligvjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ligfwq</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Day 4 of asking your opinion on a polish brand: Wet N Wild</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ligfwq/day_4_of_asking_your_opinion_on_a_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1lifxq7</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Finally I have nails long enough to showcase some polish ✨</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyfr25j2do8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1lifpfb</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈❤️🩷Alloace Pride Flag🤍💜🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lifpfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1lif5cp</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Felt appropriate for this heatwave 🔥</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lif5cp</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1liecy7</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Away from home, but the commitment to beautiful backdrops never rests</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liecy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1licom8</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1licom8/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1liclyk</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Does this look like Hema free gelpolish?</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjsbvrnmgn8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1liccjo</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>finally found my perfect nail shape 💅🏻</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liccjo</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1libzfx</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Nail Stamping by Maniology… impossible?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1libzfx/nail_stamping_by_maniology_impossible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1li5pk6</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>GF said to post here. Any care tips for my cuticles? Apparently they're in rough shape &amp; I'm not sure where to even begin.</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1li5pk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1lj1g4a</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>I don't know if i like doing chrome this way. 🤔hmm</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7clg2q3gus8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1lj3bb9</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Nail Art for Every Mood! Sophisticated Shades &amp; Bright Blooms! What do you think? 🌸 @nailsbythuyh</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj3bb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1lj2hpw</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Tips and Tricks!</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lj2hpw/tips_and_tricks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1lj2ek4</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Tiny Ramune Tamagotchi tutorial!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/24cadn934t8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1lj0w92</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Fishing Lures</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj0w92</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1lj0rbc</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Hello! As apart of my sculpting practice I do conceptual nails - I would love some feedback/advice on a work in progress set</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj0rbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1liy9a6</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Summer Solstice ✨</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejguow6g1s8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1lixvrn</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>My take on the stain glassed nails💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtizjvo6yr8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1liwgta</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Seaside Sparkle🌊✨️🦪</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liwgta</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1livyo2</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Please help me choose my vacation set 😅</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1livyo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1livr09</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Located in Tulsa! These are my favorite sets I’ve done:)</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1livr09</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1liugzo</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Any recommendation?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cu6ul6pc6r8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1lisckm</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>recent press ons i made for myself!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lisckm</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1lirzja</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Clown nails ! Yeehaw</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmi2mhmmoq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1lirk1y</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>tips about french manicure</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0puzernlq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1liqyer</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Summer Gel X Set! 🤍🐚</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liqyer</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1lilvpz</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Recommendations ?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lilvpz/recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1liln7z</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>I am a beginner that started practicing recently</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liln7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1likyn1</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>I think I have an obsession with this effect</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9z5iu2rcp8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1ligqdx</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Colors Out of Space...</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ligqdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1ligjcd</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>I did these nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ligjcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1liep0o</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>an art of encapsulated roses  🌸🌺🩷✨🦄</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1liep0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1lieja8</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>My first post 😊</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7guh2zqp0o8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1licdnq</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Newcomer help!!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1licdnq/newcomer_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1li4da8</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>I wanna snack on them 😆</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2g8g8iazk8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1lh2dlq</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>This is one of my fav set that I’ve done for my clients 😝</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t626l9tjib8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1lgorpz</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>How did I do on these??</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fi82zu7os78f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1lgi7bg</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Heavy metal vibes!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5nd3tj1268f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1lg9x7l</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>4th of July press on nails I made as a nail tech with tourrettes syndrome</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y91c48dxa48f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1lft1q9</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Blue is so in right now 😝</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqrov9dkvz7f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jun 25 08:13:30 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_29.xlsx
+++ b/data/collected_data/2025_06_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C510"/>
+  <dimension ref="A1:C713"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9103,6 +9103,3457 @@
         </is>
       </c>
     </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1ljyg9f</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Egg approves of my new nails 💅</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eiicgeghp09f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1ljxvm4</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Thoughts on the Chanel Nail Oil?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljxvm4/thoughts_on_the_chanel_nail_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1ljxnix</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Wedding nail shape</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljxnix</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1ljwoak</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Short nail press on hacks?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljwoak/short_nail_press_on_hacks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1ljwn2o</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>I made this new set today, do you like it?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j50dyrev509f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1ljwhpk</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>just wanted to share my bridal nails :)</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljwhpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1ljw8q2</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Loving my 2nd set ever!!! 🩷🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljw8q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1ljw06y</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Jungle Vibes 🌴🌺🐍</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljw06y</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1ljv91r</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Broken nail</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljv91r</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1ljvti9</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Am I getting better at painting my nails at all?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljvti9</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1ljvnbp</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Appreciation Post</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kozu6z57wz8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1ljv0a5</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Just got my abstract"4th of July" set to celebrate America</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljv0a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1ljuycx</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>What do you think of this set? I liked it a lot</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0wu39qnpz8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1ljuq6t</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Custom Soulsborne themed nails</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljuq6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1ljtram</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Everything matches here :)</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/neuelg2rez8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1ljtlk5</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>First time with gel builder</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07wcxckcdz8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1ljsxnl</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Why do my nails burn with a dremmel?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljsxnl/why_do_my_nails_burn_with_a_dremmel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1ljqmsf</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Hawaiian hibiscus 🌺 🥥🌴</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljqmsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1ljpjfd</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>My new nails! My transition set into summer sets</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljpjfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1ljqway</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Beginner here - how do I take these off?😅</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljqway/beginner_here_how_do_i_take_these_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1ljt170</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>press ons from korea!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mv9t6lme8z8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1ljsy53</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Tips to make your press ons last longer</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljsy53/tips_to_make_your_press_ons_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1ljsssu</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Scared about ring of fire</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljsssu</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1ljsof9</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>guess the price on this unlimited budget freestyle</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5yu0v085z8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1ljsc2b</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Obsessed🦋🌊🐚🌺</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljsc2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1ljs0mi</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Studio Ghibli inspired nails :3 Design vs Completion XD</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljs0mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1ljs24h</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Best way to adhere handmade press-ons?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljs24h</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1ljs44w</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>is this normal help</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljs44w</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1ljs0im</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Almost stiletto. I love 'em!</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gi5pcmezy8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1ljrprd</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Cute or too busy?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljrprd</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1ljrow0</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>New shape! Be nice, but honest, how can I improve it?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zn5b1x6owy8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1ljro3x</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Kitties and nails, the perfect combo</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljro3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1ljrngr</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>emo duck fantasy</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iik9sdvcwy8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1ljrm5x</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>New Gel X set I did today.  Gotta ward off those evil spirits!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljrm5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1ljrld5</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>juicy subtle summer set</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s19xf5ftvy8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1ljrgqs</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>New nails 💙🩵</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljrgqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1ljqzna</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>New set what are some thoughts?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljqzna</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1ljqjxp</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Got impatient and made my nails again:D</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljqjxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1ljq29m</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>a manicure especially for summer</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/955rfdwdjy8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1ljq246</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>nail cracked, how to fix?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0py01cchjy8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1ljpzgh</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Another set that took all afternoon (I'm getting faster 😉)</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljpzgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1ljpdkl</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Just wanted to celebrate my nattys</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljpdkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1ljox0a</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>I think this heat wave awakened my love for orange polish again ❤️</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhkvcvfpay8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1ljopp6</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>New nails, 💅❤</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwvn9ax69y8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1ljo2hy</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Why do my nails keep chipping?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8afqiae4y8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1ljok5d</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>recent nails i’ve done!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljok5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1ljo9vm</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>uv lamp burned my hands</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljo9vm/uv_lamp_burned_my_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1ljnhss</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>need grunge + beachy nail inspo for myrtle beach trip! getting them done tomorrow 😭💅</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kzrso260y8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1ljnd56</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>glue/ different method recommendations</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljnd56</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1ljo0ay</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Love it</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljo0ay</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1ljo07q</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Love it</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljo07q</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1ljnuao</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>How much would you guys pay for these?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/128imjzp2y8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1ljno3j</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>The right way to take a picture of your nails</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/336ns2mf1y8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1ljnb5l</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>My DIY builder gel nails</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbcakrotyx8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1ljn91q</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Got these the other day 💙</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y818peheyx8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1ljmtq9</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>nails i did for a sws and ptv concert</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljmtq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1ljmn9m</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>PAINT Nail Bar Passport Program?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljmn9m/paint_nail_bar_passport_program/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ljme7e</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>How many times in a week do I go back for a fix before I need someone money back?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljme7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ljm7rm</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Third set of press ons I’ve done!</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljm7rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ljlv3a</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Seashell nails 💅</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxi9k62qox8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ljkyzn</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Bi nails</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljkyzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1ljl60a</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Bluebies 🫐</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1n1m86wjx8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1ljkfve</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Gel toes booked for tomorrow-yellow toe nails?!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljkfve/gel_toes_booked_for_tomorrowyellow_toe_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1ljk7tg</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>let the war begin: almond or coffin?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljk7tg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1ljjr50</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Nail Repair</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dh8p9tz9ax8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1ljhi8j</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Tell me how I can improve/if I have any strong points.</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljhi8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1ljiesw</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Inside of a oyster inspired nails 🦪</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3zwt3xq71x8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ljjzil</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Just practicing</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpnj8c9tbx8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1ljj97s</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Fun new set!!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljj97s</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1ljijs1</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Is max matching a thing and is it allowed? Nails, earrings and dress all matched up for summer party! :)</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljijs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1lji8wi</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Why is this happening with my acrylic?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w0pnaczzzw8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1lji3fq</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Help on Nail Shape</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lji3fq</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1ljhugl</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Happy Birthday America 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljhugl</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1ljhm2r</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>What shape, color and length?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljhm2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1ljhjl6</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Meow 😻</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5woc3khhvw8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1ljhj0u</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Done anime samples I'm testing for a friend</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu3yxpzdvw8f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1ljhe0r</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Searching for the perfect deep red gel polish</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suso5lgguw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ljgnnx</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Glow and Glitter</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxu6no2lpw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ljgaqp</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>nail colors that work on VERY fair olive toned skin</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljgaqp/nail_colors_that_work_on_very_fair_olive_toned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1ljg9wi</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Went with a soft pink for my nails this time 💅 so happy with my natural nails and how long they’ve become</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpm16tk0nw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1ljg2uj</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Pretty pink ombré</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpopm3dolw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1ljfso5</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Soft colors</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljfso5</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1ljevko</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>I wanted summer nails, so...</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wq71ebbndw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1ljf6r3</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Neon 🌈</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljf6r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1ljfcml</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>My birthday nails 🌺</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k94necxsgw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ljfah9</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>How'd I do?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d61f9jjegw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1ljeiqz</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Pride nails + July 4th</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljeiqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ljefal</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>for my Barbie girlies here</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljefal</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1lje52w</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Are these bad</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4uj5m9o8w8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1lje2gp</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Summer nails💛🌼</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2iu9icf68w8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1ljdv1a</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>who’s 🐳y ready for summer?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yb087avp6w8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1lirg0u</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Disconnected Nail</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqy1um1xkq8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1lj5hp5</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Pls help! My nail bed is uneven, how do I fix it?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3ghlixi2u8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1lja994</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Is it normal for removal of dip to burn?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lja994/is_it_normal_for_removal_of_dip_to_burn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1ljdg42</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>how can I improve?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljdg42</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1ljaasp</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Protection on top of natural nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljaasp/protection_on_top_of_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1ljcuw0</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>How to prevent nails from snapping at finger edge?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldsie6eszv8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1ljclwh</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Clean red almond set</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdwrac24yv8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1ljcksq</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Indian here. Bornpretty nail paints ?!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ljcksq/indian_here_bornpretty_nail_paints/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ljch98</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>What shape would suit me?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27cmizn7xv8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ljydbd</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>OK I get the velvet technique now</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9himniojo09f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ljxfnq</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Sally Hansen Miracle Gel Clearance (not an ad, really)</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljxfnq/sally_hansen_miracle_gel_clearance_not_an_ad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1ljvl5r</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>how often do you switch up your manis?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljvl5r/how_often_do_you_switch_up_your_manis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1ljumak</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Dopamine in a bottle</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e2xtl46lmz8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1ljue1c</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>How do you make a watery polish thicker?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljue1c/how_do_you_make_a_watery_polish_thicker/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1ljttwy</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Does anyone else NOT like the Mooncat Getting Even Primer?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljttwy/does_anyone_else_not_like_the_mooncat_getting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1ljti5u</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Simple colors for summer?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pmj0gqicz8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1ljteze</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>I want to wear this car on my nails</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf3nd5zqbz8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1ljrbzo</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Swatch request: Tyler’s Trinkets holo glitter toppers</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuxclv1qty8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1ljqs1w</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Tried to make a jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljqs1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1ljqk2n</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>OPI Dutch Tulips</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3jby5pbny8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1ljq5qx</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>ILNP-Flip Side</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i2zq1nf7ky8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ljp8d2</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Looking for a blue + brown magnetic</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljp8d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1ljp20t</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Emily de Molly haul</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljp20t</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1ljp1gr</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Polished for Days' Room for a Thousand</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljp1gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1ljovxy</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>My technique on my shorter nails is still a bit fishy… 🐟</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kivx02hay8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1ljov5y</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Emily de Molly's Eternal Forces</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljov5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1ljoonc</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Loving this sheer pink</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljoonc</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ljmnaq</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>ISO exact dupe/shade mystery Butter London polish</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljmnaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1ljnt4c</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Need help IDing these two mystery nail polishes, Take 2</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2r153852y8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1ljnper</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Colours like &amp; Other Stories “Taffeta Silver”? (discontinued)</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db5zkgyp1y8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ljnlcp</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>My long-term relationship with Bikini So Teeny is still going strong 12 years later. 💙</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/al07cgiv0y8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ljmdtk</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Heatwave polish</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aykx1xkbsx8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1ljm41h</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Best QDTC for Magnetic Polishes</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljm41h/best_qdtc_for_magnetic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ljlyrl</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Essie- Bikini so Teeny</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd7rbjpfpx8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ljlpv0</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Mooncat - Dark Night of the Soul vs Sassy Sauce - Read Between My Tulips</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljlpv0/mooncat_dark_night_of_the_soul_vs_sassy_sauce/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ljll0k</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Trout Nails 🌈 🐟</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljll0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ljli27</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Beach Trip</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xngv29e8mx8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1ljl7s8</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Is this a close dupe for Haunted Forest by Mooncat?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljl7s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ljkrcz</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>10 days of wear - cirque colors peach jelly</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljkrcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1ljk1ii</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Mooncat primer BEFORE base coat??</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljk1ii/mooncat_primer_before_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1ljjo3l</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Londontown lakur, dazzle dry opinions</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljjo3l/londontown_lakur_dazzle_dry_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ljjfrv</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Ride or die base coat for weak nails</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljjfrv/ride_or_die_base_coat_for_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ljj5k2</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>This beauty is coming back</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljj5k2</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1ljid7w</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Happy Pride!</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljid7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ljicl6</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>My first Ethereal ft. my book!</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7kfpcps0x8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1ljib8e</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Help me find the perfect silver</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vboln73k0x8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1lji54k</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Green Polish Lovers</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lji54k</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1ljhsnk</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Red snake</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g54u27z4xw8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1ljh2dp</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>lahar 🌋</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gbbbcfwbsw8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1ljgmzv</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Cirque Colors Jellies Question</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljgmzv/cirque_colors_jellies_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1ljg7r3</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Day 5 of asking your opinion on a polish brand: OPI</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljg7r3/day_5_of_asking_your_opinion_on_a_polish_brand_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1ljg5h8</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>last set of pride nails, skittle edition!</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljg5h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1ljfx7h</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>What!?! Am I the only one?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljfx7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1ljfvyx</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Does anyone use a magnifying light?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljfvyx/does_anyone_use_a_magnifying_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1ljfsof</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Refreshing nails for the Northeast heat wave 🌬️</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljfsof</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ljfp4u</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Fixing Break in Nail?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ami5ba64jw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1ljfk3f</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈💚🤍Aroallo Pride Flag🤍💛🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljfk3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ljfi8q</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - The Polished Mage Made Me Do It!</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljfi8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1ljeipo</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>can anyone recommend a cool toned red that’s not too dark?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljeipo/can_anyone_recommend_a_cool_toned_red_thats_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1lje7jx</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Obsessed with my new Traveler’s Notebook, so painted my nails to match 💅</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lje7jx</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ljdqa0</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Probelle Nail Concealer vs Londontown Kur Illuminating Nail Concealer</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47uwrnqv5w8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ljdmh7</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Multiverse 🤗</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hdewei955w8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ljch53</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Monkey ✨✨</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljch53</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ljcc1l</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Lofi Lavender 😍😍</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljcc1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ljcaze</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Talk to me about shaping nails</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljcaze</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ljcaci</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>I know it doesn’t suit me, but look at that pink😍💖</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljcaci</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ljc59p</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>I messed up removing gel polish and I don't know how to protect my nails while they heal.</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljc59p/i_messed_up_removing_gel_polish_and_i_dont_know/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ljbk4a</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>So Needy</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljbk4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ljbeb6</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Olive coloured polish</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljbeb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ljb39h</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Lifting gel nail? What’s happening?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86bek3rwmv8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ljb34l</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Looking for Advice with Gel!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ljb34l/looking_for_advice_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ljazb0</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Hexcellent</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7c9997f1mv8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ljavvt</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>DRK Magic Effect alternative for Australians?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ac4qis9lv8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ljanhv</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Randomized super skittle</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljanhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1lja2sb</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>What do you use if you don’t like your nail polish brush?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lja2sb/what_do_you_use_if_you_dont_like_your_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1lja1dr</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Holo Taco Mani!</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fipgp79hev8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1lj7pph</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>White or clear swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lj7pph/white_or_clear_swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1lj68o8</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>I love this nail polish 😍</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj68o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1lj6ksj</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>They’re not perfect but I’m happy with them!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj6ksj</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ljzgm7</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Some recent sets ✨</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljzgm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1ljyz8b</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>How to stick metal charms to acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ljyz8b/how_to_stick_metal_charms_to_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ljudfo</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Press on nail creations</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljudfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1ljuvtl</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Beyonce’s concert nails for my girl!!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9gkmes0pz8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1ljwews</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Sparkles and Pride</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljwews</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1ljvcs0</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Press ons!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljvcs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1ljv3p5</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>New sets by @nailsbythuyh</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljv3p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1ljuuu3</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>How are you? A simple but beautiful design 😻</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76tcqghroz8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1ljum19</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>I know I want to do Something with this but not sure what: Inspo ideas?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmzp89qimz8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1ljttxh</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Celestial Sun &amp;Moon</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljttxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1ljsn0e</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Stitch and Angel nails</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljsn0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1ljslfe</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Left hand</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ku479sh4z8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1ljs8ai</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Summerween Nails</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irf5ix0c1z8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1ljs3e3</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Studio Ghibli inspired nails &gt;:3</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljs3e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1ljrgb6</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Happy Pride!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ba96lvspuy8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1ljrdgr</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>summer set i did !!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owwmp4x1uy8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1ljqokt</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Hawaiian hibiscus 🌺 🥥🌴</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljqokt</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1ljqiif</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Ok! Me piden estas uñas de cómic One Piece.</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljqiif</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1ljq26e</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Finished tamagotchi set✨</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljq26e</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1ljowz6</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Recents</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljowz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1ljn6of</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>What do you think? Some good nails. Classic and cute ✨😻</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq4vwj9yxx8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1ljmmve</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>I did a space set for myself!</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljmmve</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1ljm4ca</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Nail art for a PTV and SWS concert</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljm4ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1ljj5jk</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>I made Ice Nails</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljj5jk</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1lji6jr</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Am I being too hyper critical or should I start over?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lji6jr</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1ljhwt1</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Lobster Nails were Needed for a Trip to Maine 🦀🦐</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ljhwt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1ljhu0d</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Helppp lol</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ljhu0d/helppp_lol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1ljfmrh</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Pink Bubble Glitter</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rn4q2voiw8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1lje8gr</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Some practices</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lje8gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1ljd7ae</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Labradorite nails - multi layered approach for "embedded" or layered rainbows</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cx2xs7e92w8f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1ljb4ss</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>abstract Press-on Nails ~ | RUMISG</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmwidzytmv8f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1lja2jl</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Nails from previous week</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lja2jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1lj9n8h</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Toothless the nightfury inspired nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lj9n8h</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jun 26 08:13:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_29.xlsx
+++ b/data/collected_data/2025_06_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C713"/>
+  <dimension ref="A1:C904"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12554,6 +12554,3253 @@
         </is>
       </c>
     </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1lktlkx</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>They did my nails wrong 😭</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lktlkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1lkt761</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Hyper-realistic seashell nails !</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkt761</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1lksvi6</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Primer acid or non acid</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lksvi6/primer_acid_or_non_acid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1lkqn77</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Is this a ok combo?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwl8xbcc579f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1lkrvib</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Natural Nails Overlay</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkrvib/natural_nails_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1lkruod</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Did my nails for Emo Night :)</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkruod</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1lkrqbk</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgxbsoo2e79f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1lkronm</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>First time chrome ombre 🤘</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkronm</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1lkr9wc</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Dip nails keep chipping</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkr9wc/dip_nails_keep_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1lkr189</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Anotha one ☝️</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkr189</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1lkqxpk</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Wifey just did these for me</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkqxpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1lkqpfn</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>What shape would you call this?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu6p3yhx579f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1lkqn11</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Gel polish changing color?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkqn11</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1lkq4cx</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>honest opinions please</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkq4cx/honest_opinions_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1lkqkpo</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Gels/gel x/hard gels?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkqkpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1lkq84z</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>July 4th nails!!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkq84z</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1lkpgmi</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>How to paint better??</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkpgmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1lkpef0</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Need advice</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkpef0/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1lkpahr</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Been getting SNS/Dip for years thinking of doing press ons for a while</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkpahr/been_getting_snsdip_for_years_thinking_of_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1lkp82o</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Zebra vibes 🤍🖤</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0tm5t8zr69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1lkp5n0</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Nail lamp</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkp5n0/nail_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1lkp2wf</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>What causes lifting?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkp2wf/what_causes_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1lkoyuf</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Busted?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcxifo1lp69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1lkoncu</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>A delicate design✨</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cznpoh2qm69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1lko5yd</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>need help with weak nails</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lko5yd</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1lko0lf</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>A little Glitter</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3vx0i78h69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1lknmil</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Flavor of the week</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17s3cl4sd69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1lkngrj</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Taking advice</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scmjlobcc69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1lkmn6c</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Builder gel removal</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkmn6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1lkl6ik</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Press ons for LIFE</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkl6ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1lkn2g3</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Keep them natural?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jaur1ow869f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1lkmweq</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Some nails I’ve done on myself over the last few months!! All gel and my natural nails</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkmweq</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1lkmq8n</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Loving my engagement shoot nails (light pink on clear acrylic with white chrome)</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkmq8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1lkmpy5</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>4 week nail growth</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9liz0bw569f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1lkml5o</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Rockstar nails, from my birthday last year 🤘🏾🖤</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsj7x0ur469f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1lkmaup</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>My First Case Study</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xmh9j7b269f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1lkm9z8</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Labubu nails 🩵</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkm9z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1lklijm</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Nailbea Nails Review</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lklijm/nailbea_nails_review/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1lkkapc</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Is this discoloration a sign that my builder gel is coming off? Or is this normal?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkkapc</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1lkk7wb</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Kitty cat nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f91wvm6fl59f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1lkkfe8</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Pirate birthday nails ♥️</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkkfe8</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1lkkf6r</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>New colors.</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75okv5sym59f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1lkk9zm</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Does anyone else regret getting their nails done as soon as they leave the nail salon?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkk9zm/does_anyone_else_regret_getting_their_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1lkk9n1</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Cat Eye Diagonal French Tips</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yovfzwsl59f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1lkjxot</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>DND “cest le vie”</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkjxot</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1lkjp87</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Anyone know how to prevent summer humidity/sweat ruining my nails?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkjp87/anyone_know_how_to_prevent_summer_humiditysweat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1lkjkp8</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Advertisement gone wrong</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elgo81shg59f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1lkilwb</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Nails done professionally. I showered same day and blow dried my hair. Now the nails are yellow tipped 😭</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkilwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1lkftw8</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Nail Pain</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30a0s5pop49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1lkh37p</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkh37p</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1lkhn2h</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Why do my nails curve like this</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwom7j2b259f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1lkhs0r</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Want Gel, Don’t Want the Damage</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkhs0r/want_gel_dont_want_the_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1lkgqjw</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Green and teal on short nails</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7c9mjjzv49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1lkgf7o</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>New Set... WDYT?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/179a9k9ut49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1lkgdfk</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>I love only matt!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkgdfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1lkgdei</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Nail has weird texture</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97e1lj1ht49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1lkg8zs</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>how did you fix your brittle nails?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkg8zs/how_did_you_fix_your_brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1lkg5gq</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Tell me what I’m doing wrong</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkg5gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1lkegwv</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Can't keep a Pedi nice</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkegwv/cant_keep_a_pedi_nice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1lkc00o</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Summer flamingo set inspired by a past set on here!</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci03bpviz39f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1lkfuo7</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Decided to treat myself to a manicure and pedicure today</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a2r8f2up49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1lkfn1m</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>We’re not in kansas anymore 👀</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zsqlysaco49f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1lkfdse</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Help with my nails</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkfdse</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1lkewr4</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>The only good picture I got of my nails before I had to cut them from too many breaks =') (guy nails btw)</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gt0xej6j49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1lkeqnr</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Turned 35 today. First time I've ever gotten my nails done.</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihrh9du0i49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1lkeg3a</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Brush cleaner</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkeg3a/brush_cleaner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1lkef0t</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Dark, cozy &amp; delicate — black nails with lace for winter ❄️🖤</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkef0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1lkdzz4</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Summer Nails 💅</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkdzz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1lkdpbo</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Beginner Nail Art</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkdpbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1lkdl2e</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>My New Cirque Colors Jellies!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p85s6b6a49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1lkdjsn</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Dermacol Azure Aqua on natural nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkdjsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1lkd3mu</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Got my nails done for the beach</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nz83kqt649f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1lkcuqd</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>simple 🤍</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkcuqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1lkcqsa</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>my first time trying cat eye!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c49lq8wh449f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1lkc42s</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>What brand has Size 00 in medium almond clear press ons? Having a hard time finding! Thanks!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkc42s/what_brand_has_size_00_in_medium_almond_clear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1lkbyyi</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Obsessed 🍊🐆🌸✨</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkbyyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1lkbyas</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>My perfect red. ❤️</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkbyas</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1lkbj1v</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Something more exciting after monyhs of solid colour</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjen7spaw39f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1lkbfvi</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Essie colors for toes</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkbfvi/essie_colors_for_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1lkbeqq</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Cinnamon roll press-on nails :3 💙</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/df1fvhaiv39f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1lk8ckc</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>HELP nail broken into the nail meat what do i do??</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rewl1u3ya39f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1lkaibw</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>How can I protect my nails while I’m working?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkaibw</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1lkayla</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Jojoba oil causing peeling and breaking?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lkayla/jojoba_oil_causing_peeling_and_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1lkasqp</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Set for a Stray Kids concert</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkasqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1lk4isl</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>First time trying drugstore press ons. How bad is it?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8kkwi4xi29f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1lk3q86</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Colorful Ombre Fish Nails</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk3q86</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1lk3ofm</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Brown Summer Nails!!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr4c41wkb29f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1lk6yds</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Summer Sunset ombré Nails</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk6yds</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1lk5y4u</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Traveling for 1+ months. Please help with nail options</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lk5y4u/traveling_for_1_months_please_help_with_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1lk4k55</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Japanese gel in Japan...so gel</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lk4k55/japanese_gel_in_japanso_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1lk8x9f</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Talavera Pottery Inspired</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zulwmquxe39f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1lk9tj5</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x1n2wgozk39f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1lka7on</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Don’t usually do green but the guy I’ve gone on a couple dates with said it’s his favourite colour, so I thought it’d be fun to try!</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cbmu8imn39f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1lk9cto</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>fresh nailsss</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk9cto</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1lk8xpm</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Question…</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozo4fdd0f39f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1lk8349</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Happy Pride ❤️🧡💛💚🩵💙💜</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk8349</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1lk70jp</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>My first French manicure in 20 years!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk70jp</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1lk69o8</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Wanted to share my louboutin nails 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk69o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1lk5dw4</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Nails with black</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuu4u46sp29f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1lk5bq7</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Favorite nail file for shaping natural nails?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lk5bq7/favorite_nail_file_for_shaping_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1lktvs0</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Tectonic Shift - Mooncat</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lktvs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1lkt78s</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Help! Dry nails advice</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkt78s/help_dry_nails_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1lkri9i</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>This may win the award for ugliest polish ever.</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwwrlqr0e79f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1lkrbqa</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>What is your favorite silver linear holo polish?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkrbqa/what_is_your_favorite_silver_linear_holo_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1lkppzv</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>KISS, galaxy effects kit</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iisb14mhw69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1lkpmtt</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>SOS Builder gel</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkxkpygpv69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1lkpiwh</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Lisa Frank Pride</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkpiwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1lkp81i</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Drugstore base coats for hiding the nail line?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkp81i/drugstore_base_coats_for_hiding_the_nail_line/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1lkow8n</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer Summer Pinks</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkow8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1lkow1o</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>The only red I’ll ever need🔥</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkow1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1lkngez</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Inspired by this tiny purse</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4u8k4bh9c69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1lkn639</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>First skittle ever inspired by my daughters purse:</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkn639/first_skittle_ever_inspired_by_my_daughters_purse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1lkn60v</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>First time trying Fauve Cosmetics!</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkn60v</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1lkn5ll</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>OPI Rust and Relaxation 🍅</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqwko0wo969f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1lkmunc</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Elizabeth Rachael Fruit Art</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkmunc</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1lkmrr8</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Beyond the Reef / beyond impressed!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q4rz6knb669f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1lklzr1</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Miss Runway sparkling with flash ✨📸</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kung4scoz59f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1lkl6xo</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>It's giving "turquoise ocean water and sandy beaches" but all I have is a kiddie pool with rocks in it. (Comparisons at the end)</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkl6xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1lkl63g</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>I have this bottle of 3ina quick dry top coat but it has a dropper in it.</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkl63g</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1lkl4r2</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Similar polishes?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngdwue0ks59f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1lkkifv</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>v late pride mani</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkkifv</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1lkk5ri</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>kb shimmer must haves??</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkk5ri/kb_shimmer_must_haves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1lkk5cl</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Freshly painted Essie "Fab Florals" 🍂 Can someone help me find the gel alternative to this shade?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76uq3savk59f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1lkk127</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Day 6 of asking your opinion on a polish brand: Essie</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkk127/day_6_of_asking_your_opinion_on_a_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1lkiib1</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>I cannot figure out what the heck this brand is, helpppp</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9xlycmi859f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1lkhvec</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Help with wedding nails♥️</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkhvec</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1lkhgkn</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>need help finding this holo fish shade for my besties bday nails!!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fv6pmr1159f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1lkhd9k</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>The super-shifty beetle elytra multichrome of my dreams - KBshimmer For the Pun of It.</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iox072ef059f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1lkhba7</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>🩵💚 baja blasted 💚🩵</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkhba7</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1lkgvgo</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Recommendations for Nail polish (not gel) to match those circled in white</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkgvgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1lkgr7t</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>💙 Painted Polish Bass To The Bone 🤍</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebgn8k54w49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1lkfxx9</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Poseidon’s Prize 🧜‍♂️💙🖤💚</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8uxy9pkcq49f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1lkfsj1</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Found my powders</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9hgsy7ep49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1lkfaho</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Removers</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkfaho/removers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1lketje</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>What am I doing wrong with these velvet nails?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rta47lcji49f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1lkeowc</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>and for my next trick.....! 🪄</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mpvwp9yoh49f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1lkeeku</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Are You Floral?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3rcja3qof49f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1lkdzrk</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Doing it myself</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fydxh6owc49f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1lkdvy2</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Swatch request: Cirque - Indigo/Midnight Jellies</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkdvy2/swatch_request_cirque_indigomidnight_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1lkdoii</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Aperol Spritz</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkdoii</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1lkcu5x</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Swatches for Byte My Peach🍑?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fd90fqn2549f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1lkct6v</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>my boyfriend is horrified at how I store my nail supplies</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxbv28bw449f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1lkcjl7</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Does anyone know when/if lullaby by cirque Colors will be back in stock?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whgyqrw4349f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1lkcbhe</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Duping the vibes: Koi Whiskers</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/U4Lajjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1lkc0sy</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Dupe request!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3zsqy9oz39f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1lkbvo7</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>My perfect red.</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkbvo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1lkbq84</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Handmaids Tale inspired collection</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkbq84</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1lkb3v4</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>This sub is out here making magic and I literally cannot walk away smudge free</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkb3v4/this_sub_is_out_here_making_magic_and_i_literally/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1lkb20e</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Another post here gave me this idea and now I feel like a summery princess 👑</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkb20e</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1lkaqlp</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Octopus Games 🐙</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkaqlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1lkaerh</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Give me color, give me sparkle, give me magnetic, give me everything</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uk2ipq9po39f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1lkadrz</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Surprising polish</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqtqr9cqo39f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1lk9rki</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Watery (thermal + stamps)</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk9rki</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1lk9gfw</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Mooncat Mercury in Retrograde</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0oe4qisji39f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1lk8znf</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Infertility led me to polish 💅 What led you here?</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk8znf</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1lk8wyu</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Sparkley ✨💖✨</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8t5znorve39f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1lk8bse</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Comparison of O-Type Star and Written Invitation?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lk8bse/comparison_of_otype_star_and_written_invitation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1lk82q5</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Nail Care is Self Care!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk82q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1lk7sv2</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>I love negative space nail art &lt;3</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk7sv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1lk7d98</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>For those with oily skin, what’s your favorite base and top coat?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lk7d98/for_those_with_oily_skin_whats_your_favorite_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1lk71rv</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Summer nails🥹</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk71rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1lk6m5k</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Glossy or matte? 🌈🌵</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk6m5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1lk66mu</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Orly Kelli’s Solstice: love the color, hate the formula</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6ckhpgsv29f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1lk5sh0</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Holo Taco Toe Beans!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk5sh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1lk4nzj</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Scored this little haul for 17 USD</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3cj02olj29f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1lk4ekd</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Kaleidescope + Daydreamer</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk4ekd</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1lk49yj</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Mooncat Midnight Rider Vampiest Indigo</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk49yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1lk40t7</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Another snail, and some slugs for pride month.</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk40t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1lk2sle</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>First attempt at a ‘lazy’ gradient 🌈</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk2sle</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1lk18qi</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>My first time buying indie polish</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk18qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1lk0k9m</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>A spooky ombre between summer manis</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk0k9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1lkrx8f</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Did my nails for Emo Night :)</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkrx8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1lkri9a</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Just wanted to share :3</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkri9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1lkqw76</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Wifey just did these for me</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkqw76</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1lkqk91</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Loving this swirl French tip! What do you think of this fresh look? 💅 @nailsbythuy</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iklv1s7j479f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1lkq8pg</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Simple? @nailsbythuyh</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qq0jhtnf179f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1lkntkm</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Are you hungry? @nailsbythuys</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnesvfyif69f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1lkn0x2</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Guy nails</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkn0x2</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1lklhzx</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>New here, and just wanted to share!</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lklhzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1lkle4q</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>I did these nails for my mom, she thinks simple decorations are pretty</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5e4m5hou59f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1lkji6e</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Help.</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns2p3ymyf59f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1lkjbz3</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Estás uñas me las hice el domingo ! Son uñas en softgel . Con un brillo ojo de gato!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkjbz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1lkhfxx</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Why can't I cat eye?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lkhfxx/why_cant_i_cat_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1lkfuuc</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Polka dot nails 💕</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkfuuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1lkcx42</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Happy Pride 🌈✨</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkcx42</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1lkc99o</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Some nails I did today ❤️‍🔥💅🏼</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkc99o</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1lkc0k9</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>tips for newbiee?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkc0k9</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1lk7eu4</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>look at the design I made this week</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk7eu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1lk78dl</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Random set??? One of the favs I’ve done</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6vg4617339f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1lk61jo</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>My submission for the fishing lure trend!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xx5ygf6ru29f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1lk1xsw</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Finally got to try the fishing lure trend 🥹🎣</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lk1xsw</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jun 27 08:13:11 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_29.xlsx
+++ b/data/collected_data/2025_06_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C904"/>
+  <dimension ref="A1:C1102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15801,6 +15801,3372 @@
         </is>
       </c>
     </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1llodke</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Painted my natural nails for a change</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1llodke/painted_my_natural_nails_for_a_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1llnfr8</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Can I use a 6W lamp to cure gel on acrylics?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1llnfr8/can_i_use_a_6w_lamp_to_cure_gel_on_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1llnfkm</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>I'm a newbie, what do you think?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llnfkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1lll083</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Cutesy glitter set done by me :)</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z11spgzlee9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1llkew1</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>How should I go about filing my wonky nails if I want to grow them out?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llkew1</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1llk00i</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>My nail lady matched my nails to my bag and she popped of😍🤍</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5swlgas4e9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1llevml</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Wrinkled thumb nail beds</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llevml</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1lljcnh</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>How to fix nail split after gel x injury?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti5q6q7jyd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1lljofq</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>California destroyed my nails, what do?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lljofq</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1lljhe2</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Which do salons prefer - acrilyc nails or gel nails?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lljhe2/which_do_salons_prefer_acrilyc_nails_or_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1llja0x</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Any tips?!</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss0qlriuxd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1llg8r2</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>My works, which one you like best?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llg8r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1llhs8h</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Is this practical? Nails x Sarina on TikTok</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yalxpyi6kd9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1llivd7</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Dupes?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llivd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1llingw</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Blueberry picnic nails!</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llingw</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1llilih</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Glitter French Tips</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep5j3drird9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1llih8l</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>4th of July blues 💙</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llih8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1lli9xy</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>I wanted something simple and I’m so happy with the results!</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wa71qcplod9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1llhm3b</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Polish Ended up Being See Through and Metallic?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llhm3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1llhhgz</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>red stilettos 😽</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr279oajhd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1llhh2d</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>How can I fix my nail?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozpupaofhd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1llheg6</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>🧿</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv61fytrgd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1llhb3l</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Why ?! 😭</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94gr5stwfd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1llhalt</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Put a lil razzle dazzle on them! Done by me.💯💅🏾</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llhalt</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1llh87q</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>My newest set 😍 my nail tech called them boba tea animal mashup 🤣😍</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v13vsep6fd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1llh3xa</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>I asked how many charms she wanted, she said 'yes'</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pjgtns3ed9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1llh3ri</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>New set for my dad’s wedding 💅🏼</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8p5hk52ed9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1llh37r</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Why does this keep happening??</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llh37r</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1llh0px</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>How we feel about press ons???</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wo9uedadd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1llgzms</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Have to show the glow!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vugdo4q0dd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1llgpvv</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Is it bad to trim nails after a shower? I just started wondering if maybe that is what is making mine look damaged (peel, split sometimes)</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1llgpvv/is_it_bad_to_trim_nails_after_a_shower_i_just/</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1llgjsk</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Deep sea nails 💙 Design vs Completion &gt;:3</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llgjsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1llg27f</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Anyone knows why my nails keep breaking near the skin? They’re not even that long, still within the safe length</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llg27f</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1llg1c9</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Fourth of July Nails</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llg1c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1llfvlx</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Made some fish press ons 🐠💅</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj4h46cc3d9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1llfji9</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Japan Nails</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fniiibtk0d9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1llfaag</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>This sub made me realize I’ve been going to chop shops</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1llfaag/this_sub_made_me_realize_ive_been_going_to_chop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1lleqae</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Me after seeing that one girl paint over her girly manicure with white 💅</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oidf1zywtc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1llecbi</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Evergreen Nails 🌲💅</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ppuglvwqc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1lle5ze</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Hard gel just popped off</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lle5ze</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1lle01m</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>My cherry nails 🥹</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m44c1ia7oc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1llbi28</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>If your nails keep peeling read this‼️</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llbi28</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1lld2xb</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Black French tip with chrome</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5plgqq0hc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1llax87</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Jamberry</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1llax87/jamberry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1llcbr5</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>What is an average price?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1llcbr5/what_is_an_average_price/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1llc8be</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>First time with press on nails</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfov8rzkac9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1llc1cw</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>New setttt</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnz9gg469c9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1llbqly</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>best way to do my nails with shaky hands?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1llbqly/best_way_to_do_my_nails_with_shaky_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1llbngz</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>(repost because Reddit desktop...) fledgling still and messy but eager to go further (3rd day after application, was for Pride)</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llbngz</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1llbmfg</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>summer set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5426hhy56c9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1llbm0p</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Purple chrome forever 💜</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqfpy7b36c9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1llb7sd</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>a set my sister did, (newbie)</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx765l593c9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1llb46w</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>New nails !</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llb46w</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1llazj5</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>A lil’ vibe change to your nail feed 💅🏻</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llazj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1llaqsk</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Are my nails damaged or is this normal?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llaqsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1llaprc</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Aurora Nails! 🌌✨</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llaprc</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1llalai</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>$6 nails from target</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llalai</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1lla6zo</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Natural nail growth🫣🤯 (yes I got length took off before a new set was applied🤣)</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lla6zo</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1lla23n</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Chrome french for summer ☀️</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnpbcce1vb9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1lla14u</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Today’s set💅 compared to last summers set with the same vibe🦒</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lla14u</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ll93sh</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfgo2un9ob9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ll9z9g</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Getting into nail art!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll9z9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ll9wfo</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>My besties lil sis custom made these for me and I'm in loveeeer 😍</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll9wfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ll9tv4</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Glow</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42pvinpftb9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ll998s</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>A little something I painted on myself for pride ✨🏳️‍🌈💅</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll998s</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ll8qpn</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Did this set on my cousin</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll8qpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ll8h9n</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>First attempt at cat eye nails</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m2mldcstjb9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ll8e86</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>My builder gel won’t stop peeling the next day</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ll8e86/my_builder_gel_wont_stop_peeling_the_next_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ll87gf</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>In the mood for red ❤️</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9t21lt3yhb9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ll7nyf</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>I need lotssss Of help, I would like to get soft gel tips.. don’t mind my crusty dusty nails I just took off my uv gel tips after like 6 years…</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll7nyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1ll7u4a</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Did my nail tech do a good job ?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmcc2i0afb9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ll7pu3</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Does uv nail polish chip when playing guitar?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ll7pu3/does_uv_nail_polish_chip_when_playing_guitar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1ll7ka9</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>got these done for my birthday!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll7ka9</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1ll2vwh</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>What's the best type of nail?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ll2vwh/whats_the_best_type_of_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1ll1a08</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Dreamy Swirl Inspo by Kaomitl on Insta!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll1a08</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1ll2m44</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Opinion on red nails</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ll2m44/opinion_on_red_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ll563v</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Are my gel nails too thick? Hi m</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll563v</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ll6gs4</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Going back and forth between canceling my Russian Manicure appointment</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll6gs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1ll765j</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>I did these with regular polish!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4uwjvfnab9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ll6ztw</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>hating and loving them</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mqkxfkh9b9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ll6wnt</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Press on nails- yay or nay?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n4cok1w8b9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ll6uy8</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>This weeks nails on my girlfriend. Hand painted sardines by moi</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll6uy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ll6gih</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Summer Gingham Set</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hezxqiu5b9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ll66ib</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>First time !</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2juu45zx3b9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ll5rxu</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Obsessed with my nail tech’s work on my nails.</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll5rxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ll5aqf</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>1 month clean of nail biting. Not sure how to manage.</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll5aqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ll4zj0</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jzg3sorva9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ll44yn</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Got nails done first time in forever</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ogc0vwvupa9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ll4265</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>I asked my husband to pick my polish for his birthday this weekend and this is what he chose💚🖤</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll4265</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ll40i0</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Are my nails too short to get builder gel (from a salon)?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cuiahlyoa9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ll3jbs</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Dip progress - thank you &amp; welcome further pointers &lt;3</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll3jbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ll366y</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Is it pretty or not? Be honest</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll366y</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ll2xwc</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>two broken nails before mani pedi thursday 😭</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll2xwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ll2u1s</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>First nails done by myself ✨</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll2u1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ll25cf</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Old Navy</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll25cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ll23kt</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Pride Nails ✨</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9y31ejglba9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ll1wnf</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Nail tech delivered but I’m not loving the color scheme I choose</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wj5vqmz7aa9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ll1ke5</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>first time doing isolated chrome 💕</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86xnyj0r7a9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ll14f0</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>🗣️ You know I A.T.E</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcls4hch4a9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ll0z1u</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Got asked if they were press ons!!!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf7hux8c3a9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1llm92k</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Did I take off my Gel X wrong?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llm92k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1lllflz</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Starry Night Swatch</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/01mnyrj0je9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1lljw3x</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Can you tell if a polish will stain?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lljw3x/can_you_tell_if_a_polish_will_stain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1llj7rh</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>How to care for a nail split from gel injury?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbkoxw0axd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1lli93s</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Kanebo Kate Dupe?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q07z3cqlnd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1llhxjr</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Tried my hand at making my nails look like a wizard’s hat</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll9kg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1llggo2</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Anyone wear press ons while working?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1llggo2/anyone_wear_press_ons_while_working/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1llh6r6</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>How often do your nails break?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1llh6r6/how_often_do_your_nails_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1llh458</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Day 7 of asking your opinion on a polish brand: Revlon</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1llh458/day_7_of_asking_your_opinion_on_a_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1llgkpf</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>I need help editing my ILNP cart, big list below</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1llgkpf/i_need_help_editing_my_ilnp_cart_big_list_below/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1llgann</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>My 3 year old made me a “cake”</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18cl6dpy6d9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1llfz70</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Baby's first thermal!</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llfz70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1llfz3c</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>i know a lot of people are going to be very happy about this!!!</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xt2q3q864d9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1llfisw</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Looking for jelly polishes with scattered large flakies like this PPU polish from April</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehdy6dff0d9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1llfe6h</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Charmed pumpkin and Calcifer</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llfe6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1llf3zv</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>How to clean brushes/lids</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id421mm1xc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1lleskz</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Bridget🧡❤️</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lleskz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1llelmi</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Wild Berry Skittles</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llelmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1llehzh</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>EDM's shimmer toppers are *amazing*</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llehzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1llehh0</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Follow Your Dreams</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llehh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1lle5kx</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Btartbox hot love ❤️</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhzbhd30pc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1lldocx</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Holos are hard…</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2v54lmpglc9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1lldo0w</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Manimod drawer inserts all the same size for Bisley?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqyy0x9llc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1lldkjs</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>jelly hibiscus 🌺🧡🏝️</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lldkjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1lldhvg</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Glisten &amp; Glow is doing their 25% off summer sale</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8z1svor8kc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1lld98a</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Any female born after 1983 Can’t Cook, All They Know Is Mcdonalds, Charge Their Phone, Twerk, Be Bisexual, Eat Hot Chip And Lie</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tis4yqmeic9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1lld0ll</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Help me pick a polish for vacation</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lld0ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1llc1x2</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Think I just duped myself - KB Shimmer Present Tense vs Lurid Indomitable</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llc1x2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1llbshb</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>L.A. Colors Neon Jelly</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llbshb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1llbeqy</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Horseshoe magnet deal!</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/dp/B0DT3KNC43?ref=cm_sw_r_apin_dp_CJQK9A5E3H3G7ZE24ER0_2&amp;ref_=cm_sw_r_apin_dp_CJQK9A5E3H3G7ZE24ER0_2&amp;social_share=cm_sw_r_apin_dp_CJQK9A5E3H3G7ZE24ER0_2&amp;previewDohEventScheduleTesting=C&amp;csmig=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1llbccz</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>has ANYONE been able to find a long nail keyboard cover that isn't for a mac?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1llbccz/has_anyone_been_able_to_find_a_long_nail_keyboard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1lla43b</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>We all know about lip combos - what about nail combos?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lla43b/we_all_know_about_lip_combos_what_about_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1ll9yqg</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>PSA: BKL vault polishes 30% off</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ll9yqg/psa_bkl_vault_polishes_30_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1ll908a</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>BKL Windcaller</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyauw7pknb9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ll8pod</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>What is a BKL mystery polish?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkzcl8rhlb9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ll8p40</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>💙 ILNP Bluebell 💛</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll8p40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ll8ki7</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>June Stamps</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll8ki7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1ll8dvf</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Best super pigmented, one coat gold and silver for nail art</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ll8dvf/best_super_pigmented_one_coat_gold_and_silver_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1ll7t5z</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>How to stop these chips</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unnyx7t3fb9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1ll7o6n</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>FINALLY TRIED ESSIE GEL COUTURE</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ll7o6n/finally_tried_essie_gel_couture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1ll6vs0</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>What a STEAL😍</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc98lbvp8b9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1ll6piw</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Be who you aaarrrreee for your priiiddee 🏳️‍🌈🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll6piw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1ll6mk5</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>ILNP polish in “Unraveled” 🤭</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll6mk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1ll6g5u</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Throwbacks</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ll6g5u/throwbacks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1ll665x</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Bug nails 😍 🐛🐞 🐝</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll665x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1ll5pjd</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Should I make this my next mani?</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cou0jvur0b9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1ll5m4w</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>What's your best dupe for Serpents of Eden?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95119p4bza9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ll4br3</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Let this be a lesson, not all sheers are meant to be worn alone! before &amp; after</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll4br3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1ll45b0</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Does anyone know a dupe of this color in acrylic powder?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6qfk8wwpa9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ll3832</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>DISO Gelaze Pink Voltage Product or Dupe</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll3832</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ll35zb</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Dupes for Sinful Colors Sheer Mattes?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll35zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ll2rhz</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>The most ethereal polish in my collection</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxqat1c9ga9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ll2aei</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Apparently this “doesn’t count as packing for vacation”</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll2aei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ll28jc</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Thinking Cool Thoughts</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll28jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ll27p8</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Finally got around to buying &amp; hanging polish racks and it’s so satisfying</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/19BWdS3.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1ll2253</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Fishing Lure nails 💅 🐠💚</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll213q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1ll21w0</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>1-week-old cat eye still looking sharp and crisp!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll21w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ll1erh</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Inspired by the other bikini so teeny posts</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll1erh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ll1a1e</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Help! I only wear one colour and it’s running out</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll1a1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ll0jp5</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Mooncat Marshmallow</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll0jp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ll0gf6</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈💛🤍Non-binaryPride Flag💜🖤🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll0gf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ll03dn</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Rare(?) Swatch Pic Style</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yj2f86shw99f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1lkzz32</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Not perfect, but Im really happy with them!</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaltapojv99f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1lkzf68</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Blurring Base coats</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkzf68/blurring_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1lkyzjk</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Essie - Handmade With Love</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkyzjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1lkyzgy</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Cracked Polish - Anywhoozers</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkyzgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1lkyvew</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Happy little bluebirds</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/518shhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1lky7v0</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>My first holographic nails ever</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lky7v0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1lky2gv</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Vacation Nail Inspo</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lky2gv/vacation_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1lkw5mp</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Peeling nails - no escape from gloves</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkw5mp/peeling_nails_no_escape_from_gloves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1lksgi0</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>cheapest top coats</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lksgi0/cheapest_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1lkw6o9</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>ILNP Jellies and Blurring Base Coats</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lkw6o9/ilnp_jellies_and_blurring_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1llo4et</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>my second time posting here, did these on myself✨️</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llo4et</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1lln1bj</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>HELP ME PICK BIRTHDAY NAILS :)</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lln1bj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1llkh6m</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Summer frenchies!!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsrm2die9e9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1lljptx</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Channel Your Inner Beyoncé: "Cowboy Carter" World Tour Nails Event! @nailsbythuyh</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ds24r7rz1e9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1llha22</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>My newest set 😍 my nail tech @nails_emmywynn called them boba tea animal mashup 🐆🧋</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3yuzs7nfd9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1llfhwx</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>I loved this design I made today.</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgsia1280d9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1lle633</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Flores que se hacen solas.</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhbrxm67pc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1lle1s4</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>syrup gel recs?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lle1s4/syrup_gel_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1lldj15</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Fruit and Creepy Crawlers</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/til7d3whkc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1llczfk</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Nails 💅🏾 by @Beuty_antto_ar</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/el7cyqsagc9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1llcqpy</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>some fav press on sets i’ve made recently! :-)</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llcqpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1llcjfk</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>I did my nails myself since my nail tech is in the hospital (shes okey btw)</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llcjfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1llbx69</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>🔥</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4an8pg7b8c9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ll8tt9</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Handmade 420 nail set + magnetic bear charm that really works 🐻🔥</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll8tt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ll8tox</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Nails in Madrid</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j2yv80aamb9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ll8c1o</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Old Navy</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll8c1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ll6wu1</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>I suck at doing magnetic gel, I just seem to always disperse the particles and they disappear. Are you guys doing 1 or 2 coats, and using the magnet on both coats (if doing two)?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ll6wu1/i_suck_at_doing_magnetic_gel_i_just_seem_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ll4tjr</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Aura nails🌞💐🧡</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3aipkamua9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ll4rzf</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>FEW MOREEEE</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v22m9cbbua9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ll4ro3</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>This was an easier set than I was expecting😩💚very colorful for summer vibes 🏖️🌊</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80ob7rx8ua9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1ll4qi2</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Just started my nail art journey 💅 | Would love your feedback on my latest Pinterest-inspired sets!</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll4qi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1ll3ymj</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Obsessed 🍊🐆🌸✨</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ll3ymj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ll0xph</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>💛💛</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0s5uj623a9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ll094l</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>New set with flowers, gold lines and rhinestones</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q1btcaqx99f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1lkyqcq</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Who puts lemons in a fruit salad? Ew.</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bx6h5je0l99f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1lkx3be</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>fruity vibes 🍓🍉🫐🍋🍒</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lkx3be</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun 28 08:11:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_29.xlsx
+++ b/data/collected_data/2025_06_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1102"/>
+  <dimension ref="A1:C1307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19167,6 +19167,3491 @@
         </is>
       </c>
     </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1lmh91w</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>🔥🔥🔥🔥</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmh91w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1lmh8li</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>It’s giving peach 🍑 @nailzbypriya</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7159g242im9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1lmh5qu</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Clean, filed and ready for paint!</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9i5v3ku4hm9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1lmh5l5</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Cute short nail set - @nailzbypriya</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmh5l5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1lmh0lk</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>This month's set. First time attempting French nails.</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmh0lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1lmfv0t</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Just trying to blend in with the leaves 🍂</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/113i3gs42m9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1lmfozr</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Nail Archive 🌸</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmfozr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1lmeusz</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>found my new fav gel colour 💜</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns9x6ozxql9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1lmeiqh</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Finally reach my nail length goal!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fspyh4gnl9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1lmek4e</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>How to achieve this color/design?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmek4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1lmamfz</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Damaged nails?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw5d2dtqkk9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1lmb919</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>how do i start with builder gel?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmb919/how_do_i_start_with_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1lmbrzq</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmbrzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1lmc5he</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Glamnetic and Showering</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmc5he/glamnetic_and_showering/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1lmdae0</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Birthday set</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmdae0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1lmebo3</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>🩷❤️</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pbh7ivdll9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1lme76t</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>You know it's time for a new mani when...</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lme76t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1lmcx3f</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>An lemony set I made last year 🥰</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80e4ce0y6l9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1lmchdw</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Im getting a new manicure tomorrow. What would you suggest?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qk9hdsbk2l9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1lmc64v</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Does this shape look good on me?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5mhf9lgzk9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1lmc3l3</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>The classic french fringe will never go out of style</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjftgwenyk9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1lmbxsn</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>what can i do to stop my french tips from chipping 😔</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmbxsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1lmbqh8</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Newest press-on set that I'm obsessed with 🌈 like $6</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmbqh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1lmbdur</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Hawt Dawgs</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85nxt9byrk9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1lmah7c</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>1 year growth natural nails</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7tj7qrdjk9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1lma6a5</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Concave nail sizing :/</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4ot1wpzmgk9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1lm9y4j</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>i loveeee my tech</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm9y4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1lm9sao</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Unfamiliar E file bits....</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm9sao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1lm95ut</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Getting manicures</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm95ut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1lm9s06</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>First summer set of the season 💕</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm9s06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1lm9l9f</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Strawberry nails 🍓</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm9l9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1lm9pkt</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>my most perfect manicure !</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sco8qdbck9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1lm9g44</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Month almost two month update</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm9g44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1lm9fl3</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Nice set today</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phgeb0oz9k9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1lm9alg</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Happy Cancer szn 🌊</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wnd9k7ap8k9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1lm986r</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Garden in blume</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm986r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1lm957k</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>A bit of whimsy ✨</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bh34goch7k9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1lm9485</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅 🥳</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm9485</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1lm9295</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>4th of July nails!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5i76ypq6k9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1lm90p8</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Should I be charged for a nail repair</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lm90p8/should_i_be_charged_for_a_nail_repair/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1lm894e</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>What would be the difference in booking a “shellac manicure with add-in builder gel overlay”, and “full set bio gel and shellac” when booking a nail service?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lm894e/what_would_be_the_difference_in_booking_a_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1lm7zss</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Loving these foils ✨</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpf8vousxj9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1lm7yz1</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Can I still get a set of acrylics????</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm7yz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1lm7y9u</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>I did my 'Murica nails for the 4th.</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd8ws1kfxj9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1lm7swf</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wf50ama8wj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1lm7nvn</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>How do we feel about this blue color??</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4odxfzr5vj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1lm6dw2</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>First time getting square nails and I am surprised by how much I love them</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm6dw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1lm64vc</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>When your inspo is simply “fish queen” and your tech delivers 😂</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eksvm72bjj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1lm6u4v</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>I did my nails again!! My toes are also navy blue 😩🙏</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm6u4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1lm6skf</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I love pink</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nm9zue9oj9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1lm68zo</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>i need help 😢</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cacnaio5kj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1lm67gw</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Mermaid nails for summer🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f70y89ujj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1lm5wtq</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Let my lil sis practice nails on me, felt fabulous! 😂</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tkmh00lhj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1lm5vd9</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>How to prevent lifting at the free edge 😭</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lm5vd9/how_to_prevent_lifting_at_the_free_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1lm5sgn</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Opinion on set?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yoem59sngj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1lm5glg</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Got these nails at today!</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm5glg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1lm5qqy</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>UF-Glow by Polished For Days</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gim2zclagj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1lm5hm8</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>my new design</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09te93bbej9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1lm502d</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Finally able to do my nails again!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1dalvtlaj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1lm4kk3</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Ringing in summer with these bad girls</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45gg64ub7j9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1lm4fru</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>I’m at a place that I’m happy with my natural nails (finally)</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wi1wzzn96j9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1lm4fev</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Want to try my own gel nails…any advice appreciated!</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lm4fev/want_to_try_my_own_gel_nailsany_advice_appreciated/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1lm4bak</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Gel X - do these look normal? should I go back to acrylic??</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm4bak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1lm3znn</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Is it normal to bleed for 20 mins after a manicure?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lm3znn/is_it_normal_to_bleed_for_20_mins_after_a_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1lm3q44</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>My nail stuff💅🏼</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3l3meby31j9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1lm3s5t</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Always drawn towards going green🌲💚</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm3s5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1lm3gpi</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Pink Lemonade Vibes</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mk95t48zi9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1lm3gej</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>y2k summer set my nail tech did for me 😍🌞🌺</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf6jzve5zi9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1lm3dha</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Where are my animal print girlies?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm3dha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1lm390c</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Would love feedback and suggestions!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm390c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1lm34dv</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>I'm 54 and straight. The color/design matches my personality</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm34dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1lm339z</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>On our way to the beach and this is how it starts 😩😩</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqorblnewi9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1lm2mya</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Junk nails but make it pink candy</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1ur2es0ti9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1lm2eqm</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>my cute nails</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tlwtogfri9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1lm1quh</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>A month of growth and cuticle care</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm1quh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1lm1nqo</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>I don’t know if this is the right place for this but..what colour should I do?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7u0h4yzli9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1lm1c16</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Supposed to get a dip fill today..</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1s86kj5qji9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1lm19ov</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>🍒Cherry nails🍒</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q3ipo99ji9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1llzvsq</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>can i use a uv top coat to protect my glamnetics?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llzvsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1lm02bo</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Pretty changes Barbie set</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm02bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1llzpc5</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>birthday nails 🥳</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nr50iiz7i9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1llzmsz</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Hand-sculpted 3d Vegas nails!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llzmsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1llzis4</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>taste the rainbow 🌈 (last few month’s sets)</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llzis4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1llzhrr</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>My nails princess by @nailsroom999</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9y0l58h6i9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1llyill</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>onycholysis - help?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nu2f76mzh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1llyhql</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Tried French for the first time</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llyhql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1llz5as</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>30 years old, first ever nail appointment in a week. What should I even ask for?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llz5as</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1llp56a</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>How do I strengthen my nails</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1llp56a/how_do_i_strengthen_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1llpjmi</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>What nail shape would fit on my hand?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llpjmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1llvkm7</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Some recents!</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llvkm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1llywbu</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>BIAB, Korean jelly polish, and some daisies 🌼</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hupz33b0i9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1llyg6x</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>I love getting holiday nails 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3wq5ul0zh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1lly9v6</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Rainbow skittles for pride month</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lly9v6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1llxuet</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Should I cut my natural Nails?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llxuet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1llxr5c</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Am I being dramatic to want this thumb fixed?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llxr5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1llxqhh</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>New summer set!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llxqhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1llxjzm</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>I love little gems on my nails but hate when this happens. Is it me, is it normal, or is it the quality of the embellishments?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5ihwerwsh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1llx51d</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Perfect nails for summer!</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llx51d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1llx03x</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>First time getting long nails</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vshs5clxoh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1lltq9e</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>finger tips swell from at-home gel polish</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lltq9e/finger_tips_swell_from_athome_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1lmhjaw</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>3am manicures</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmhjaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1lmggfb</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>im a newbie and having trouble making my nails look professional</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/593zyvvw8m9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1lmfvo0</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>ISO a purple polish w/red flakies and/or glitter</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lmfvo0/iso_a_purple_polish_wred_flakies_andor_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1lmfmyx</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Would love help and comments on my ILNP cart</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmfmyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1lmfm4y</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Cracked Polish HELP!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lmfm4y/cracked_polish_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1lmf0zm</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Polished For Days “Lush” over OPI “Russian Navy”</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzrzu8qrsl9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1lmecqk</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Blue for July</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmecqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1lmeanw</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Feeling realllllly proud of my Ghibli mani</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhzfh1yyjl9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1lmdy6g</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>I made a Ride the Cyclone skittle!</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3c3gqz0fhl9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1lmdwrk</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Red Velvet ❤️</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmdwrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1lmd7y1</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Pretty Indie Brand</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmd7y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1lmd4s5</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Ok yall i'm hoping for a miracle</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmd4s5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1lmd2pn</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>In looove with this bright cherry red for summer</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4h57d64k8l9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1lmc0y6</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>cuticle oil and hand cream recommendations?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lmc0y6/cuticle_oil_and_hand_cream_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1lmbw14</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Last manicure for the month.</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmbw14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1lmb85o</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Chrome powder experiment</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrqga8ifqk9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1lmayfc</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Please excuse my haggard hands! Too many rainy days, so I put on some fun to counter.</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5tspxjjvnk9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1lmawkh</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Athymy- GITD!</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmawkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1lmam1z</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Pearlescent/Shimmery Gold? Dupe for O+J’s Sunlit</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkgam15nkk9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1lma515</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Sunscreen dulling polish?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lma515/sunscreen_dulling_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1lm9u5w</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Stars ✨</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/se3izioldk9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1lm9fi4</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Stella Chroma - Sangria</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm9fi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1lm99k2</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Living adventurously!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/230bxd6j8k9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1lm8t5t</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Help!  Been looking forever  for a bright or neon red that does  NOT have any orange.  Suggestions?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lm8t5t/help_been_looking_forever_for_a_bright_or_neon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1lm8o8o</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>But why????</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87p40sqg3k9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1lm8d5s</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>I love it when people buy me gifts but why do they have to be dupes 🥲</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm8d5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1lm8cvq</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Attempting to create a Ride the Cyclone skittle!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwrj9pss0k9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1lm8chv</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Two aspects of Emily de Molly - Leave a Light On, plus a dupe attempt</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jkd43epo0k9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1lm6en9</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Can't wait to swatch my first ILNP haul!</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm6en9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1lm644w</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Impressed by how glowy Ghoulish is indoors</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03s89yylij9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1lm5k77</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>UF Glow by Polished For Days</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2hf2ex8vej9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1lm5fjk</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Bright pink AND glow in the dark? Yes please!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm5fjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1lm57pc</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>very late pride mani!</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm57pc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1lm4ybg</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>I rarely paint my nails,however fell in love with this one while looking for a gift for my friend</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39vxag79aj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1lm4xvt</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Finally reach my nail length goal</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g99ul9v5aj9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1lm4quk</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>BKL Earth Sunderer</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm4quk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1lm4mdl</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Dupe Request: Labradorite by Dany Vianna</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm4mdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1lm445p</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Looking for updated opinions on OPI’s Repair Mode</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lm445p/looking_for_updated_opinions_on_opis_repair_mode/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1lm3sd0</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>How Do I Achieve This Look?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jf9ayzpk1j9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1lm3ghq</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Behold! My most prettiest, most lovely, most fabulous nails to date! 💅🥹</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm3ghq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1lm2tea</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Glow in the dark!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pr55inpdui9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1lm1sm9</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>I’m So Bluuuue!</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm1sm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1lm1oob</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Can i put a top coat over my gel nails if it broke like this?</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fuc1pqf7mi9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1lly04y</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Bubble Gum Blue &amp; Pink Barry</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tg3oj5svh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1lm1e9q</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Broken / Not yet broken bottle - What to do?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm19nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1lm18c1</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Willow Wisp by Daveen Lacquer OBSESSED</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm18c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1lm165l</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I don’t love cremes but I can get down with a pink in any shape or form</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ish6jm4iii9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1lm12pb</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>You know her, you love her (and she's coming back in July!)</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm12pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1lm0mw9</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Looking for a wearable gold!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lm0mw9/looking_for_a_wearable_gold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1lm0mss</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>A little bit of improvement</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4lpix4mei9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1lm0eqq</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Obsessed 😍</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm0eqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1lm04n4</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Growth Help!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm04n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1lm0176</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Willow Wisp</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm0176</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1llzy83</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Somebody said they wanted to see polish in hospital lighting?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llzy83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1llzqg3</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>My deco beauty stickers wore away during the night</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llzqg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1llyx1k</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>ILNP Brownstone</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/semrrudf2i9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1llyl34</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Brand new acetone bottle not sealed?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llyl34</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1lly81s</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Summer beach vibes ✨️</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td84m5ikxh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1lljtbb</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Vintage-ish mauve-y taupe Dupe/ID request</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lljtbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1llxwi3</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Flower Child as a topper 💙</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llxwi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1llxpzb</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Pleased with my haul (scratching the Mooncat itch)</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxkauyqarh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1llxjpq</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; Co Cherry Blossom</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5ub6v8psh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1llxchh</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Almost too late for my rainbow pride nails but I got them in on time!</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llxchh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1llx8dx</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Shelves meant for coffee bars are great for hanging swatch sticks!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llx8dx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1llx6j5</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>I'm in love with this glitter polish ❤️</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv7yesc6qh9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1llwwh7</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer brushes</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1llwwh7/night_owl_lacquer_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1llwuyy</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>What's your favorite yellow?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llwuyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1llwhun</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Danny Phantom Themed Interlocking Dotticure :)</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llwhun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1llvlbd</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Lavender Haze</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igvsgjpreh9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1llvkg3</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Umm Bog Dweller what?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1llvkg3/umm_bog_dweller_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1llvhna</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Nail polish and Skin Undertone?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1llvhna/nail_polish_and_skin_undertone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1llvch7</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Nails with Teaspoon: Cadillaquer Orchid and Zoya Yohannah</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jhtw4xxch9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1llv6fa</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>When you love your nail polish so much you have to do a whole ass nature photo shoot</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llv6fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1lluj24</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>I've done it with this subreddits' help</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jsa7ons6h9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1lluf7m</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Any advice/help on Sally Hansen Good Cheer-y</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lluf7m/any_advicehelp_on_sally_hansen_good_cheery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1llu90u</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Another winner from Lurid</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llu90u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1lltyrz</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Indomitable and Riding Sleeping Bags are the polish of dreams</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lltyrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1llt2vk</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Why is the top coat nail polish at the tip of my nails turning cloudy?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzowtfyvug9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1llrvs9</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Little magnet case</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llrvs9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1llrnyp</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>What nail polish color would you wear with this dress for a wedding?</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1r41ykwohg9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1llq1ri</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>better late than never. happy pride!</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/787wctkdyf9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1lmgrxt</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Can’t get nail foils to stick</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lmgrxt/cant_get_nail_foils_to_stick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1lmg8mt</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Gemstone nail art 💎</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n1tu6doe6m9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1lmf8t4</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>picnic nails 🧺💐🐞</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmf8t4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1lme46n</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Golden Tide✨️🌊🐠</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lme46n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1lmcsc8</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Fishing Lure Nails</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmcsc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1lmcked</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Loving this soft coral base with delicate 3D florals. What do you think? @nailsbythuyh</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61p3daec3l9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1lmc7nx</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>funky press-ons</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmc7nx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1lmb9pf</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>El anillo de serpiente 🐍 queda?</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9o9mhrgqk9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1lmawlh</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>hi i need help finding a good nude base color! mainly for when i do french tips, pictured is a color i like so anything similar! beetles only sales this polish in a very tiny bottle in a bundle with other colors that i dont need &lt;/3</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmawlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1lm865i</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>lil olive set i finished! :,)</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm865i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1lm61pa</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Let my lil sister get some nail art practice 😅</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ta16hh9mij9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1lm4dst</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Strange question..</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lm4dst/strange_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1lm3gcg</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Aurora nails! 🌌✨</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm3gcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1lm2ztd</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Disappointed with these stickers 🙁</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm2ztd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1lm0lrs</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>A set I made for my bestie💜</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm0lrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1lm01ak</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Pretty Changes Barbie set</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lm01ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1llwlb5</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Tips on fixing this?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llwlb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1llvqld</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Magnetic bear nail charm actually holding a joint 🐻💅💨</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ldvf7zjufh9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1llupom</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>First attempt at junk nails</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llupom</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1llunyl</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Hi, I'm a noob and wanted tips on using mirror powders.</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1llunyl/hi_im_a_noob_and_wanted_tips_on_using_mirror/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1llt9pf</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Something fun for her vacation ✨ Swipe for her Back to School set 💜</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llt9pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1llt0ly</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Lavender 💜</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llt0ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1llovt4</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Just got my nails done, had to share it with you all!</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swgsxl3umf9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1llor7g</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>The Limoncello ones</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1llor7g</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun 29 08:11:07 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_06_29.xlsx
+++ b/data/collected_data/2025_06_29.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1307"/>
+  <dimension ref="A1:C1489"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22652,6 +22652,3100 @@
         </is>
       </c>
     </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1ln99tt</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>First time DIY gel manicure</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln99tt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1ln8vjg</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>First time having nailss</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9ov55s7kt9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1ln8g9n</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>4th of July glitter ombre</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dp138oubft9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1ln8fdl</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Neon</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ava99o1ft9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1ln85cv</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>🐍🐍🐍🐍</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/janf2l3sbt9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ln7q3n</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Just a man who tried press-ons for the first time + first time I tried painting/stoning nails too ^-^"</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3a6ozhs6t9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ln7plz</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db6a6l0n6t9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1lmlfu4</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Nailboo nail glue caused my natural nail to rip off</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmlfu4/nailboo_nail_glue_caused_my_natural_nail_to_rip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1lmoq09</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Nail glue papeles types my nails</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j03de474mo9f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1ln6dmz</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>My first set ever!!</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln6dmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1ln6hp2</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>kinda random but i wanted to share these cause i think theyre cool :)</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nl0wljb1ts9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1ln6hf5</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Nails I did on myself tonight :)</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77j97oryss9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1ln6dby</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Limoncello nails 🍋🍸🐡 DIY press-ons</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln6dby</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1ln5wdu</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>confused about the way my nails were done today</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3crjmlbkms9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1ln5lp5</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>he chose purple, not sure why tho 😅🎮</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzjseccljs9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1ln5k5v</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Waiver</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcu883n5js9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1ln4ssp</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Is it bad for your real nails to get gel manis/pedis every month?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ln4ssp/is_it_bad_for_your_real_nails_to_get_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1ln50zx</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Do you guys think it’d be okay for me to get another full set? Ugh i need my nails</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/799kunuods9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1ln5ayk</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>This is my 2nd attempt using the Manicurist (Paris) set. I’ve never done my own nails before so I’m pretty happy with the results 😊</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln5ayk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1ln53sh</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>When there's a storm outside, the idea comes unexpectedly.</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/he364nsbes9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ln4ygc</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>4th of July</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krrt8diycs9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ln4w9q</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>4th of july nails!</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln4w9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1ln4vj1</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>How bad are these? Lifelong nailbiter trying to fix it</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln4vj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1ln47gh</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln47gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1ln4710</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>In the sunlight😍✨</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g0qqdpg85s9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1ln44yf</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Feel like this red is too warm for me…? colour theory/undertones are real 😭</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtq0p0jn4s9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1ln43cm</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Currently ☺️💙💚✨</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t66nfg134s9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1ln42bv</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Got my nails done today and I think they are bad.</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln42bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1ln2mp8</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>When you want to do extensions but the process goes wrong every step of the way so you just chop them off and slap on a full coverage color 😡😭</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ok2yv1xpr9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1ln3g9h</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Nail care/extension question?</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3dzirnsxr9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1ln2yvy</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Went to a new salon today after my last set turned out horribly at my old regular salon …needless to say 10/10</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln2yvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1ln2qyg</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Love my new nails</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arkxcchzqr9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1ln2p36</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>😭</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nd1sf9kqr9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1ln21bq</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Did my husband's nails</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln21bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1lmzhah</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>My nail is detaching??</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmzhah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1ln0kmd</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Did my nails</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln0kmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1ln149z</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Before and After: 15 months of dry manicures with hard gel</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln149z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1ln20ge</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>🫧 New set I love it so bad 💕</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvaoyjl8kr9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1ln1wwv</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Tropicana Daze</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln1wwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1ln1n77</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Freehand 🩶</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfzlv4wtgr9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1ln1k1t</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Almond or sharp square?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln1k1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1ln0gor</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Pre-painted Press ons Adhesion</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ln0gor/prepainted_press_ons_adhesion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1ln0mzf</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>This hello kitty is off to Hawaii</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln0mzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1ln0mvi</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Super simple but I’m so happy with how much better my cuticle work has gotten 🎀</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln0mvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1ln0mpc</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>This hello kitty is off to Hawaii</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln0mpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1lmzg3e</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Hard Gel Nails Hurting, Need Advice</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmzg3e/hard_gel_nails_hurting_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1lmzvj5</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>polka dot fun! 🌈🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/toowus061r9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1lmzre1</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>My two favorite things together…</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmzre1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1lmzdxr</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>One of my fav sets 🌼 🐝</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1jt03tkywq9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1lmzcdf</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Natural nails not covered by my nail tech?</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dx5gvw6iwq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1lmza1e</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Summer fruit nails 🍉🍒🍓</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmza1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1lmz5lt</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Been getting my nails done since I was 14 - Now 33. Just get acrylic overlay. My nail tech is 🙌🏽🙌🏽</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxuk1lz0vq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1lmz29r</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Yellow frenchies with flowers 💛🌼</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmz29r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1lmz1lo</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>My subtle pride nails</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c0x98n2uq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1lmywes</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Vacation cat eye 😎</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s56q6svvsq9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1lmynl4</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Pride Nails 🌈</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zj6lzuhtqq9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1lmyl6h</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Shockingly, claws this long aren't very keyboard-compatible</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmyl6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1lmyk6q</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>can I get just nail art done on my gel x extensions?</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmyk6q/can_i_get_just_nail_art_done_on_my_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1lmyj01</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Babyboomer nails 💅</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmyj01</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1lmyibt</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Nail Growth Progress + Manicure Journey ✨💅</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmyibt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1lmy3bd</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>New Nail Place</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmy3bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1lmxyqk</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>On the hunt for this color</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22vvn5u6lq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1lmxy9h</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Red with lightning.</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmxy9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1lmxt6g</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Pressons</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmxt6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1lmxqzq</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Showing off my natural nails</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odjm554fjq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1lmxo74</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>New Salon who dis?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmxo74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1lmxmpu</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Ive been doing nails my whole life and would love to become a nail tech but theres some things holding me back</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmxmpu/ive_been_doing_nails_my_whole_life_and_would_love/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1lmxm7b</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>I was told I have tiny nail beds</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmxm7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1lmxb72</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>My nails are vacation ready 🚢</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tt4ljsufq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1lmxavj</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Best shape?</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmxavj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1lmwx4o</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>DIY Chrome/Shimmer for BIAB</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmwx4o/diy_chromeshimmer_for_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1lmweep</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>french &lt;3</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmweep</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1lmvzrw</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>silver chrome I got done today!</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djg4zupb5q9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1lmvzqn</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Just got my nails done !❤️💛💚💙💜</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmvzqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1lmvyu7</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Is this an average length for a man's nails?</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yirnyji45q9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1lmvx4x</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Cruella inspired nails</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmvx4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1lmvhrg</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Which should I get?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmvhrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1lmvcfx</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>What HEMA free press on glue have people been using?</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmvcfx/what_hema_free_press_on_glue_have_people_been/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1lmurg5</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Nails Hurting After Hard Gel Manicure</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmurg5/nails_hurting_after_hard_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1lmuk98</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>I tried capturing The Kiss on my ring finger in my first set of press-ons^^</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmuk98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1lmvwpu</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Ombré pink and black almond shape</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5ic0c5o4q9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1lmvw6w</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Winner thank you!</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02l7rzoj4q9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1lmvm48</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Summer Vacay Nails!!</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yz1f8p3c2q9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1lmvjob</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Manicure not included with nail enhancement?</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmvjob/manicure_not_included_with_nail_enhancement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1lmvhxg</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Russian mani on natural nails 💅</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmvhxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1lmvcdg</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Cutting acrylic nails</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmvcdg/cutting_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1lmv2ym</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Best gel base &amp; top coat?</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vc0ybbz4yp9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1lmv0we</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>My first time trying French tips with a little design 🌸</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmv0we</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1lmuvsq</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Best YouTube/tiktoks to learn?</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmuvsq/best_youtubetiktoks_to_learn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1lmus7z</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>First time doing CatEye Gel!</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kujsqosvp9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1lmuof8</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Finished my first semester of nursing school and IMMEDIATELY ran to the salon.</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isaze6yzup9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1lmulh9</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>A set I made to celebrate the holiday~</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmulh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1lmuhtl</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rwrqzkmtp9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1lmud42</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>ILNP Alice flashing in the sunlight ✨</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d6o5b7dlsp9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1lmu1ew</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7h55mt4qp9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1lmty3t</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Just me, or...is this not very good work?</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmty3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1lmklen</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Olive oil in a bottle hack</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmklen/olive_oil_in_a_bottle_hack/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1lmtzxq</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Purple ⭐️✨ and 🌙</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmtzxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1lmokjs</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>E-file for gel nails at home. Good/Bad Idea?</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lmokjs/efile_for_gel_nails_at_home_goodbad_idea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1lmq3ji</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>First time acrylics - a little irritation</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmq3ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1ln9e3o</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Half Year 2 2025 - Wear all my colour polishes</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixwchcvlqt9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1ln8fj4</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>All the magic things!</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln8fj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1ln5ypt</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Similar formulas?</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3pgqn2ens9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1ln5nk3</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Second attempt at a cat eye...</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lgx5ubz5ks9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1ln5h81</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>I unintentionally bought Cosmo and Wanda</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68hpkgqdis9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1ln5da0</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>My lacquersona is a stranger to me</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ln5da0/my_lacquersona_is_a_stranger_to_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1ln49cy</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>ILNP dotted nail art  🌈</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln49cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1ln44we</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>my first cracked order came in!!!</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln44we</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1ln3tea</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>💀down in the underworld💀</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v4r1yhfd1s9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1ln1qmx</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Making lemonade 🍋 🧊 ✨</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln1qmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1ln1p0k</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Finally scratched the itch</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/707k2f6ahr9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1ln1ktv</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Polished for Days Doom Buggy</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln1ktv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1lmzxld</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Clionadh vaporwave: any pics?</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/duil43cn1r9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1lmzx5q</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>polka dot fun! 🌈🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5df6aulj1r9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1lmzvs8</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Got builder gel under my nail, help?</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckwi1v481r9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1lmzoug</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Pan pride 💗💛💙</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hutw4jkzq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1lmzmo3</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>A simple rainbow gradient never gets old 🌈🌟</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmht7zd2zq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1lmz8y5</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>We Never Lie About Bunnies, Bunny</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hx6hwx61vq9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1lmz8xh</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>any tips on how to make my nails and nail designs look neater?</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmz8xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1lmz1ch</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Mooncat’s “Outlaw Country” + silver jewelry 🩶💍🪙</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjbckbl0uq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1lmyc3o</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Mooncat’s Heart of Stone</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmyc3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1lmyapw</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Slippery Little 🐍</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmyapw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1lmy64x</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Mixing acetones</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lmy64x/mixing_acetones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1lmy33s</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>New releases from Olive Ave Polish</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/646clob6mq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1lmy0w4</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Tectonic shift 🪩</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu970cdkkq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1lmxe68</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Turn it up to Eleven at the beach</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lmxe68/turn_it_up_to_eleven_at_the_beach/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1lmwuqy</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>My Glitter Placement Birthday Nails! ✨🧁</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmwuqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1lmwdsj</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>sstarss</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmwdsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1lmvpxm</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>We all have that one polish…</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/57o6zvw23q9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1lmvg62</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Flower child 💐</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmvg62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1lmv9a7</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>BKL Appreciation</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmv9a7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1lmv7k9</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Lynb — If You Musk</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmv7k9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1lmspyy</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Suggestions for whitening natural nail tips?</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lmspyy/suggestions_for_whitening_natural_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1lmuvfd</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Ok! Fancy Gloss!!</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmuvfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1lmul4x</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>As good as I expected 🩷❤️💜</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmul4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1lmuiqh</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Loving! Tropical Heatwave -Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmuiqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1lmua4b</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Ex nail biter</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmua4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1lmu7dq</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>ILNP Alice velvetized</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hspk9lvdrp9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1lmu29u</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Do you know a polish like the base of this mani?</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4vuml7bqp9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1lmu03w</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>(almost) finished my swatch book!!</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmu03w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1lmtlf3</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Old Solar Polishes</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmtlf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1lmtjwu</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>🐚Sea Ya Later🐚</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gfo5px6mp9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1lmt0fd</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Zoom meetings for days</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmt0fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1lms4qy</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>First time with magnets</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lms4qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1lmrlob</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Oversized Bow 🎀</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmrlob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1lmr5d0</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Can the ugly polish be redeemed? 🤔</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq4nortc4p9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1lmq3yf</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Impromptu nail photo shoot on a rainy-day run 💧🌺 ✨</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmq3yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1lmpsa6</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>I‘m really proud of these</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmpsa6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1lmo53f</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>My Pride Nails!</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cjbul1leo9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1lmo215</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>🥰Glitter gel stilettos🖤</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmo215</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1lmo0a3</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>More Monster than Monster</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xhy3zcigo9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1lmnug4</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Not sure why I waited to try this one 🧚🏼‍♂️</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmnug4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1lmnrtj</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Love layering some toppers because I’m extra extra</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmnrtj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1lmnqzh</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>KBShimmer Isle Be There Topper</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/970glqnheo9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1lmnp1d</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>My first ILNP order!</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmnp1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1lmnk0l</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>my updated polish storage!!</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmnk0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1lmnhpt</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Today's combo</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmnhpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1lmn5hh</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈Progress Pride Flag🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmn5hh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1lmlv0p</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>GPL Living in Captivity</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9hus1e3yn9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1lmlh7m</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Bees Knees UP polish</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmlh7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1lmflvv</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>First mani ever</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lmflvv/first_mani_ever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1lml9hz</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Peachy 🍑</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lml9hz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1lml7jy</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Lovers to Enemies</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wv30a4qrn9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1lmjz0s</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Waimea or Bust✨🩵💚✨</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0cac6huten9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1lmjwn8</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Red jellies</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmjwn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1lmjm9x</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>0.5 gal, pls drop a tutorial</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmjm9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1lmjgpt</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>ILNP Amber vs. KBShimmer Jupiter</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lmjgpt/ilnp_amber_vs_kbshimmer_jupiter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1lmicd0</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Is this ragebait or would it work? Any pros or scientists here?</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eyfc6d1ovm9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1ln9btc</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>I think those are really cute💋</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7m32cwgupt9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1ln98yv</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Made some koi fishes</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln98yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1ln8jv7</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Man nails.</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln8jv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1ln3wc9</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Set for Stray Kids Chicago performance</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln3wc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1ln13sk</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Wanted to hop on this trend</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln13sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1ln0nl6</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Super simple but I’m so happy with how much better my cuticle work has gotten 🎀</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ln0nl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1ln0209</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Did some stamping on my natural nails</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03yo2p2p2r9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1lmxh6d</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>First attempt at isolated chrome</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e34qgw27hq9f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1lmwutz</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Steady hands when trying designs</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ak9zfk79cq9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1lmupwf</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>Strawberry/strawberry jam inspired nails!</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmupwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1lmsxyx</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Sliver cateye gel x extensions🩶</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnl7s3pthp9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1lmr628</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Tok’r Torch 💅🔥 My magnetic joint holder nail charm 2.0 drop</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lho39kbi4p9f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1lmn7py</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Not patriotic, but I love a theme...</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lmn7py</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1lml2jg</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>Press on set by me :)</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lml2jg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>